<commit_message>
V1.2 MAJOR RELEASE: INJURIES, FULL SPREAD MODEL, AUTOMATIC TWEET GENERATOR, AND HUGE DATA COLLECTION OF PLAYER GAME LOGS
</commit_message>
<xml_diff>
--- a/current_games_total.xlsx
+++ b/current_games_total.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>year</t>
   </si>
@@ -91,52 +91,49 @@
     <t>ratings_2k</t>
   </si>
   <si>
+    <t>calc_over_prob</t>
+  </si>
+  <si>
+    <t>Orlando</t>
+  </si>
+  <si>
     <t>Detroit</t>
   </si>
   <si>
-    <t>LAClippers</t>
-  </si>
-  <si>
     <t>Chicago</t>
   </si>
   <si>
-    <t>Brooklyn</t>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Portland</t>
+  </si>
+  <si>
+    <t>Sacramento</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Milwaukee</t>
+  </si>
+  <si>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
   </si>
   <si>
     <t>SanAntonio</t>
   </si>
   <si>
-    <t>Denver</t>
-  </si>
-  <si>
-    <t>Portland</t>
-  </si>
-  <si>
-    <t>LALakers</t>
-  </si>
-  <si>
-    <t>NewYork</t>
-  </si>
-  <si>
-    <t>Houston</t>
-  </si>
-  <si>
-    <t>GoldenState</t>
-  </si>
-  <si>
-    <t>OklahomaCity</t>
-  </si>
-  <si>
-    <t>Sacramento</t>
-  </si>
-  <si>
-    <t>Orlando</t>
-  </si>
-  <si>
-    <t>Dallas</t>
-  </si>
-  <si>
-    <t>Philadelphia</t>
+    <t>Memphis</t>
   </si>
 </sst>
 </file>
@@ -494,13 +491,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:27">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -576,8 +573,11 @@
       <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:27">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -585,67 +585,76 @@
         <v>2023</v>
       </c>
       <c r="D2">
-        <v>225</v>
-      </c>
-      <c r="E2">
-        <v>8099286</v>
+        <v>230</v>
       </c>
       <c r="F2">
-        <v>113.175429726997</v>
+        <v>114.722479185939</v>
       </c>
       <c r="G2">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I2" t="s">
         <v>33</v>
       </c>
       <c r="J2">
-        <v>0.5560975609756098</v>
+        <v>0.5171717171717172</v>
       </c>
       <c r="K2">
-        <v>98.31081900910009</v>
+        <v>98.42509250693803</v>
       </c>
       <c r="L2">
-        <v>114.1428715874621</v>
+        <v>115.8052728954672</v>
       </c>
       <c r="M2">
-        <v>116.2273761375126</v>
+        <v>114.4395004625347</v>
       </c>
       <c r="N2">
-        <v>75.71311931243679</v>
+        <v>77.55603607770584</v>
       </c>
       <c r="O2">
-        <v>0.3824759858442871</v>
+        <v>0.4198704902867715</v>
       </c>
       <c r="P2">
-        <v>0.5629711830131447</v>
+        <v>0.5908640148011101</v>
       </c>
       <c r="Q2">
-        <v>0.3002692113245703</v>
+        <v>0.2783799722479186</v>
       </c>
       <c r="R2">
-        <v>11.67899393326593</v>
+        <v>12.37654949121184</v>
       </c>
       <c r="S2">
-        <v>11.77815975733064</v>
+        <v>11.5350138760407</v>
       </c>
       <c r="T2">
-        <v>0.2264265672396359</v>
+        <v>0.2105568917668825</v>
       </c>
       <c r="U2">
-        <v>0.9936385401843456</v>
+        <v>1.005455558158974</v>
       </c>
       <c r="V2">
-        <v>1.02969706452677</v>
+        <v>1.038430802510143</v>
       </c>
       <c r="W2">
-        <v>11.68878638026398</v>
+        <v>10.46283211763107</v>
+      </c>
+      <c r="X2">
+        <v>0.557123034227567</v>
+      </c>
+      <c r="Y2">
+        <v>40.5</v>
+      </c>
+      <c r="Z2">
+        <v>76.59999999999999</v>
+      </c>
+      <c r="AA2">
+        <v>0.4936169592900065</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:27">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -653,67 +662,76 @@
         <v>2023</v>
       </c>
       <c r="D3">
-        <v>221.5</v>
-      </c>
-      <c r="E3">
-        <v>18126939</v>
+        <v>236</v>
       </c>
       <c r="F3">
-        <v>109.2121212121212</v>
+        <v>112.2164855072464</v>
       </c>
       <c r="G3">
-        <v>9.5</v>
+        <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I3" t="s">
         <v>34</v>
       </c>
       <c r="J3">
-        <v>0.4431818181818182</v>
+        <v>0.5372340425531915</v>
       </c>
       <c r="K3">
-        <v>97.88955627705627</v>
+        <v>98.93817934782609</v>
       </c>
       <c r="L3">
-        <v>111.024512987013</v>
+        <v>112.646240942029</v>
       </c>
       <c r="M3">
-        <v>115.465367965368</v>
+        <v>115.878125</v>
       </c>
       <c r="N3">
-        <v>76.39507575757575</v>
+        <v>76.05253623188406</v>
       </c>
       <c r="O3">
-        <v>0.3974523809523809</v>
+        <v>0.4087871376811594</v>
       </c>
       <c r="P3">
-        <v>0.5611109307359309</v>
+        <v>0.5646467391304347</v>
       </c>
       <c r="Q3">
-        <v>0.2842900432900433</v>
+        <v>0.2813088768115942</v>
       </c>
       <c r="R3">
-        <v>13.41580086580086</v>
+        <v>12.52803442028986</v>
       </c>
       <c r="S3">
-        <v>11.68452380952381</v>
+        <v>11.2513134057971</v>
       </c>
       <c r="T3">
-        <v>0.2122489177489177</v>
+        <v>0.2089909420289855</v>
       </c>
       <c r="U3">
-        <v>0.9588421528720036</v>
+        <v>0.9834924233763924</v>
       </c>
       <c r="V3">
-        <v>0.9904268292682927</v>
+        <v>1.01876925814006</v>
       </c>
       <c r="W3">
-        <v>10.89788037769227</v>
+        <v>11.46413181898958</v>
+      </c>
+      <c r="X3">
+        <v>0.4402173913043478</v>
+      </c>
+      <c r="Y3">
+        <v>41.5</v>
+      </c>
+      <c r="Z3">
+        <v>75.15000000000001</v>
+      </c>
+      <c r="AA3">
+        <v>0.5349346164410206</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:27">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -721,67 +739,76 @@
         <v>2023</v>
       </c>
       <c r="D4">
-        <v>238</v>
-      </c>
-      <c r="E4">
-        <v>39292623.5</v>
+        <v>239.5</v>
       </c>
       <c r="F4">
-        <v>115.7245293466224</v>
+        <v>115.3787234042553</v>
       </c>
       <c r="G4">
-        <v>4.5</v>
+        <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
         <v>35</v>
       </c>
       <c r="J4">
-        <v>0.5368689733408962</v>
+        <v>0.531678486997636</v>
       </c>
       <c r="K4">
-        <v>100.249446290144</v>
+        <v>99.58307328605201</v>
       </c>
       <c r="L4">
-        <v>114.4070874861573</v>
+        <v>114.6597163120567</v>
       </c>
       <c r="M4">
-        <v>115.0600775193799</v>
+        <v>114.905011820331</v>
       </c>
       <c r="N4">
-        <v>77.04465669988925</v>
+        <v>76.71513002364065</v>
       </c>
       <c r="O4">
-        <v>0.4083330564784053</v>
+        <v>0.3341248226950354</v>
       </c>
       <c r="P4">
-        <v>0.590956533776301</v>
+        <v>0.5818765957446808</v>
       </c>
       <c r="Q4">
-        <v>0.2419017165005538</v>
+        <v>0.248455791962175</v>
       </c>
       <c r="R4">
-        <v>12.94363233665559</v>
+        <v>11.37695035460993</v>
       </c>
       <c r="S4">
-        <v>12.39772978959026</v>
+        <v>12.54451536643026</v>
       </c>
       <c r="T4">
-        <v>0.2062332502768549</v>
+        <v>0.2077384160756502</v>
       </c>
       <c r="U4">
-        <v>1.01601869487816</v>
+        <v>1.011207041229232</v>
       </c>
       <c r="V4">
-        <v>0.9554474545975149</v>
+        <v>1.09050101759209</v>
       </c>
       <c r="W4">
-        <v>11.29039968385036</v>
+        <v>10.71066028731968</v>
+      </c>
+      <c r="X4">
+        <v>0.4886524822695035</v>
+      </c>
+      <c r="Y4">
+        <v>44</v>
+      </c>
+      <c r="Z4">
+        <v>76.59999999999999</v>
+      </c>
+      <c r="AA4">
+        <v>0.478910851199879</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:27">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -789,67 +816,76 @@
         <v>2023</v>
       </c>
       <c r="D5">
-        <v>230</v>
-      </c>
-      <c r="E5">
-        <v>12140852</v>
+        <v>234</v>
       </c>
       <c r="F5">
-        <v>115.5388542257516</v>
+        <v>112.4932065217391</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s">
         <v>36</v>
       </c>
       <c r="J5">
-        <v>0.5212705615428247</v>
+        <v>0.4895833333333334</v>
       </c>
       <c r="K5">
-        <v>99.26072036301758</v>
+        <v>99.61326992753621</v>
       </c>
       <c r="L5">
-        <v>115.4482132728304</v>
+        <v>112.5564764492754</v>
       </c>
       <c r="M5">
-        <v>113.3429948950652</v>
+        <v>116.633786231884</v>
       </c>
       <c r="N5">
-        <v>73.57458876914349</v>
+        <v>74.7070652173913</v>
       </c>
       <c r="O5">
-        <v>0.3678037436188316</v>
+        <v>0.3866417572463768</v>
       </c>
       <c r="P5">
-        <v>0.592251843448667</v>
+        <v>0.5744692028985507</v>
       </c>
       <c r="Q5">
-        <v>0.247200510493477</v>
+        <v>0.2839759963768115</v>
       </c>
       <c r="R5">
-        <v>12.22163925127623</v>
+        <v>13.71272644927536</v>
       </c>
       <c r="S5">
-        <v>13.02178105501985</v>
+        <v>12.50629528985507</v>
       </c>
       <c r="T5">
-        <v>0.2108560692002269</v>
+        <v>0.2192010869565217</v>
       </c>
       <c r="U5">
-        <v>1.014388535783596</v>
+        <v>0.9859176732843044</v>
       </c>
       <c r="V5">
-        <v>0.9742526722571291</v>
+        <v>1.055318573668062</v>
       </c>
       <c r="W5">
-        <v>11.84495801366901</v>
+        <v>10.84714287100455</v>
+      </c>
+      <c r="X5">
+        <v>0.358695652173913</v>
+      </c>
+      <c r="Y5">
+        <v>36.5</v>
+      </c>
+      <c r="Z5">
+        <v>74.7</v>
+      </c>
+      <c r="AA5">
+        <v>0.5008239892537384</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:27">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -857,67 +893,76 @@
         <v>2023</v>
       </c>
       <c r="D6">
-        <v>246.5</v>
-      </c>
-      <c r="E6">
-        <v>12589436.5</v>
+        <v>239</v>
       </c>
       <c r="F6">
-        <v>116.074021554169</v>
+        <v>115.0423360833695</v>
       </c>
       <c r="G6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I6" t="s">
         <v>37</v>
       </c>
       <c r="J6">
-        <v>0.5548780487804879</v>
+        <v>0.5472074468085106</v>
       </c>
       <c r="K6">
-        <v>100.9369256948383</v>
+        <v>99.76076856274423</v>
       </c>
       <c r="L6">
-        <v>114.7602382302893</v>
+        <v>114.3002605297438</v>
       </c>
       <c r="M6">
-        <v>117.8955473624504</v>
+        <v>117.0547546678246</v>
       </c>
       <c r="N6">
-        <v>76.47946681792399</v>
+        <v>75.2677811550152</v>
       </c>
       <c r="O6">
-        <v>0.3858403289846851</v>
+        <v>0.402405557967868</v>
       </c>
       <c r="P6">
-        <v>0.5847195121951219</v>
+        <v>0.5686847590099871</v>
       </c>
       <c r="Q6">
-        <v>0.2643806012478729</v>
+        <v>0.2626880156317847</v>
       </c>
       <c r="R6">
-        <v>12.90986954055587</v>
+        <v>12.07757273122015</v>
       </c>
       <c r="S6">
-        <v>12.29171866137266</v>
+        <v>12.12581415544942</v>
       </c>
       <c r="T6">
-        <v>0.2047643221781056</v>
+        <v>0.2098382544507164</v>
       </c>
       <c r="U6">
-        <v>1.019087107587086</v>
+        <v>1.008258861379224</v>
       </c>
       <c r="V6">
-        <v>1.09704211456892</v>
+        <v>1.043698859086146</v>
       </c>
       <c r="W6">
-        <v>11.4821514385633</v>
+        <v>10.76685529504964</v>
+      </c>
+      <c r="X6">
+        <v>0.383195831524099</v>
+      </c>
+      <c r="Y6">
+        <v>29</v>
+      </c>
+      <c r="Z6">
+        <v>74.94999999999999</v>
+      </c>
+      <c r="AA6">
+        <v>0.5169201007426152</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:27">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -925,67 +970,76 @@
         <v>2023</v>
       </c>
       <c r="D7">
-        <v>234</v>
-      </c>
-      <c r="E7">
-        <v>5890104.5</v>
+        <v>241</v>
       </c>
       <c r="F7">
-        <v>113.6744186046512</v>
+        <v>112.804347826087</v>
       </c>
       <c r="G7">
-        <v>10.5</v>
+        <v>8</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I7" t="s">
         <v>38</v>
       </c>
       <c r="J7">
-        <v>0.4941927990708478</v>
+        <v>0.5227272727272727</v>
       </c>
       <c r="K7">
-        <v>98.04401993355481</v>
+        <v>98.79999999999998</v>
       </c>
       <c r="L7">
-        <v>115.4636489479513</v>
+        <v>113.9260869565217</v>
       </c>
       <c r="M7">
-        <v>115.3819767441861</v>
+        <v>118.2184782608696</v>
       </c>
       <c r="N7">
-        <v>77.01962901439647</v>
+        <v>75.9891304347826</v>
       </c>
       <c r="O7">
-        <v>0.3619598560354375</v>
+        <v>0.3754347826086956</v>
       </c>
       <c r="P7">
-        <v>0.5929122369878184</v>
+        <v>0.5772934782608695</v>
       </c>
       <c r="Q7">
-        <v>0.2793635105204872</v>
+        <v>0.2719891304347826</v>
       </c>
       <c r="R7">
-        <v>13.12234219269103</v>
+        <v>13.15543478260869</v>
       </c>
       <c r="S7">
-        <v>11.86381506090808</v>
+        <v>11.91413043478261</v>
       </c>
       <c r="T7">
-        <v>0.2126579457364341</v>
+        <v>0.2077445652173913</v>
       </c>
       <c r="U7">
-        <v>0.9980194785307389</v>
+        <v>0.988644590938536</v>
       </c>
       <c r="V7">
-        <v>1.012492682355696</v>
+        <v>0.9914098480645845</v>
       </c>
       <c r="W7">
-        <v>9.813258624054932</v>
+        <v>11.52216595171919</v>
+      </c>
+      <c r="X7">
+        <v>0.3804347826086957</v>
+      </c>
+      <c r="Y7">
+        <v>31</v>
+      </c>
+      <c r="Z7">
+        <v>74.15000000000001</v>
+      </c>
+      <c r="AA7">
+        <v>0.4977575470846392</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:27">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -993,132 +1047,73 @@
         <v>2023</v>
       </c>
       <c r="D8">
-        <v>225.5</v>
-      </c>
-      <c r="E8">
-        <v>8826403</v>
+        <v>246.5</v>
       </c>
       <c r="F8">
-        <v>112.5487012987013</v>
+        <v>118.7065217391304</v>
       </c>
       <c r="G8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I8" t="s">
         <v>39</v>
       </c>
       <c r="J8">
-        <v>0.5090909090909091</v>
+        <v>0.5</v>
       </c>
       <c r="K8">
-        <v>96.14908008658008</v>
+        <v>100.8882367149758</v>
       </c>
       <c r="L8">
-        <v>115.8262445887446</v>
+        <v>117.3172946859904</v>
       </c>
       <c r="M8">
-        <v>115.3954545454545</v>
+        <v>113.2206280193237</v>
       </c>
       <c r="N8">
-        <v>76.50254329004329</v>
+        <v>77.02420289855073</v>
       </c>
       <c r="O8">
-        <v>0.4458906926406926</v>
+        <v>0.38692922705314</v>
       </c>
       <c r="P8">
-        <v>0.5933457792207792</v>
+        <v>0.5855654589371981</v>
       </c>
       <c r="Q8">
-        <v>0.310862554112554</v>
+        <v>0.2835183574879227</v>
       </c>
       <c r="R8">
-        <v>12.34350649350649</v>
+        <v>11.81096618357488</v>
       </c>
       <c r="S8">
-        <v>11.95459956709957</v>
+        <v>12.19275362318841</v>
       </c>
       <c r="T8">
-        <v>0.2279916125541126</v>
+        <v>0.2119192028985507</v>
       </c>
       <c r="U8">
-        <v>0.9881360956865786</v>
+        <v>1.040372670807453</v>
       </c>
       <c r="V8">
-        <v>1.027684152770722</v>
+        <v>0.9925325042687567</v>
       </c>
       <c r="W8">
-        <v>11.89533132535269</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>2023</v>
-      </c>
-      <c r="D9">
-        <v>234</v>
-      </c>
-      <c r="E9">
-        <v>30123535</v>
-      </c>
-      <c r="F9">
-        <v>115.2142857142857</v>
-      </c>
-      <c r="G9">
-        <v>3.5</v>
-      </c>
-      <c r="H9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9">
-        <v>0.5952380952380952</v>
-      </c>
-      <c r="K9">
-        <v>99.42738095238093</v>
-      </c>
-      <c r="L9">
-        <v>114.6642857142857</v>
-      </c>
-      <c r="M9">
-        <v>113.4559523809524</v>
-      </c>
-      <c r="N9">
-        <v>76.54285714285712</v>
-      </c>
-      <c r="O9">
-        <v>0.3706785714285714</v>
-      </c>
-      <c r="P9">
-        <v>0.5896309523809524</v>
-      </c>
-      <c r="Q9">
-        <v>0.2860595238095238</v>
-      </c>
-      <c r="R9">
-        <v>12.39285714285714</v>
-      </c>
-      <c r="S9">
-        <v>12.06904761904762</v>
-      </c>
-      <c r="T9">
-        <v>0.2155119047619047</v>
-      </c>
-      <c r="U9">
-        <v>1.011538943935783</v>
-      </c>
-      <c r="V9">
-        <v>1.069516633037821</v>
-      </c>
-      <c r="W9">
-        <v>11.52929342789112</v>
+        <v>11.72748061756648</v>
+      </c>
+      <c r="X8">
+        <v>0.6258454106280193</v>
+      </c>
+      <c r="Y8">
+        <v>42</v>
+      </c>
+      <c r="Z8">
+        <v>75.55000000000001</v>
+      </c>
+      <c r="AA8">
+        <v>0.4889823474744299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>